<commit_message>
feat: model accuracy is checked, persona is explicitly broken into continuous and discrete for better clarity
</commit_message>
<xml_diff>
--- a/data/customer.xlsx
+++ b/data/customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Surojit Mondal\Desktop\sbi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A30DE0-EAB8-47C3-BEF5-C97EB5BE4945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32EFC9-918E-4986-9638-D62184BB6C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8186,7 +8186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2370" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2395" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2401" sqref="A2401"/>
     </sheetView>
   </sheetViews>

</xml_diff>